<commit_message>
kareoke style for stories
</commit_message>
<xml_diff>
--- a/backend/الغزوات.xlsx
+++ b/backend/الغزوات.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f58b35e40015d4ae/سطح المكتب/Raya.github.io/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="11_B8ACEE991895064A1CB304B4C4E8A0A449CCCB21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11EF1636-04E0-4C41-B4B4-B1D518A0CF59}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="11_B8ACEE991895064A1CB304B4C4E8A0A449CCCB21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9C964DF-CACD-4D66-8F6F-4B013FD6E3D4}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3059,8 +3059,8 @@
   </sheetPr>
   <dimension ref="A1:AD1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1037" sqref="L1037"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
change the story header banner background
</commit_message>
<xml_diff>
--- a/backend/الغزوات.xlsx
+++ b/backend/الغزوات.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f58b35e40015d4ae/سطح المكتب/Raya.github.io/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="402" documentId="11_B8ACEE991895064A1CB304B4C4E8A0A449CCCB21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86DC1A95-C94D-49F0-BA0D-17CB18DEE68A}"/>
+  <xr:revisionPtr revIDLastSave="432" documentId="11_B8ACEE991895064A1CB304B4C4E8A0A449CCCB21" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A6D969C1-BCC3-4BF0-B0D4-87A5043B8F4E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -110,7 +110,7 @@
     <t>غير محدد</t>
   </si>
   <si>
-    <t>فِي شَهْرِ صَفَرٍ مِنَ السَّنَةِ الثَّانِيَةِ لِلْهِجْرَةِ، خَرَجَ رَسُولُ اللهِ بِنَفْسِهِ فِي أُوْلَى غَزَوَاتِهِ، وَكَانَ مَعَهُ سَبْعُونَ رَجُلًا مِنَ الْمُهَاجِرِينَ. وَقَدِ اسْتَخْلَفَ النَّبِيُّ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ عَلَى الْمَدِينَةِ سَعْدَ بْنَ عُبَادَةَ رضي الله عنه، ثُمَّ تَوَجَّهَ النَّبِيُّ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ بِالْجَيْشِ لِيَعْتَرِضَ قَافِلَةً لِقُرَيْشٍ كَانَتْ تَمُرُّ بِتِلْكَ الْمَنَاطِقِ. وَصَلَ الجَيْشُ إِلَى مَنْطِقَةِ وُدَّان (وَتُسَمَّى أَيْضًا الأَبْواء)، وَلَكِنَّهُمْ لَمْ يَلْقَوْا قَافِلَةً وَلَا حَدَثَ قِتَالٌ. وَفِي هَذِهِ الْغَزْوَةِ، عَقَدَ رَسُولُ اللهِ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ مُعَاهَدَةَ أَمْنٍ وَسِلْمٍ مَعَ بَنِي ضَمْرَةَ، وَكَانَ سَيِّدُهُمْ يُدْعَى عَمْرُو بْنُ مَخْشِيٍّ الضَّمْرِيِّ. وَقَدْ نَصَّتِ الْمُعَاهَدَةُ عَلَى: أَنْ يَكُونَ بَيْنَ الْمُسْلِمِينَ وَبَنِي ضَمْرَةَ أَمْنٌ وَسِلْمٌ. وَأَنْ لَا يُنَاصِرُوا أَعْدَاءَ النَّبِيِّ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ . وَإِذَا احْتَاجَ النَّبِيُّ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ إِلَى نُصْرَتِهِمْ، فَإِنَّهُمْ يَنْصُرُونَهُ. وَكَانَ لِوَاءُ الغَزْوَةِ أَبْيَضَ، وَقَدْ حَمَلَهُ حَمْزَةُ بْنُ عَبْدِ الْمُطَّلِبِ رضي الله عنه. وَدَامَتِ الغَزْوَةُ خَمْسَةَ عَشَرَ يَوْمًا، ثُمَّ رَجَعَ رَسُولُ اللهِ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ وَمَنْ مَعَهُ إِلَى الْمَدِينَةِ.</t>
+    <t>فِي شَهْرِ صَفَرٍ مِنَ السَّنَةِ الثَّانِيَةِ لِلْهِجْرَةِ، خَرَجَ رَسُولُ اللهِ بِنَفْسِهِ فِي أُوْلَى الغَزَوَات، وَكَانَ مَعَهُ سَبْعُونَ رَجُلًا مِنَ الْمُهَاجِرِينَ. وَقَدِ اسْتَخْلَفَ النَّبِيُّ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ عَلَى الْمَدِينَةِ سَعْدَ بْنَ عُبَادَةَ رضي الله عنه، ثُمَّ تَوَجَّهَ النَّبِيُّ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ بِالْجَيْشِ لِيَعْتَرِضَ قَافِلَةً لِقُرَيْشٍ كَانَتْ تَمُرُّ بِتِلْكَ الْمَنَاطِقِ. وَصَلَ الجَيْشُ إِلَى مَنْطِقَةِ وُدَّان (وَتُسَمَّى أَيْضًا الأَبْواء)، وَلَكِنَّهُمْ لَمْ يَلْقَوْا قَافِلَةً وَلَم يَحدُث قِتَالٌ. وَفِي هَذِهِ الْغَزْوَةِ، عَقَدَ رَسُولُ اللهِ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ مُعَاهَدَةَ أَمْنٍ وَسِلْمٍ مَعَ بَنِي ضَمْرَةَ، وَكَانَ سَيِّدُهُمْ يُدْعَى عَمْرُو بْنُ مَخْشِيٍّ الضَّمْرِيِّ. وَقَدْ نَصَّتِ الْمُعَاهَدَةُ عَلَى: أَنْ يَكُونَ بَيْنَ الْمُسْلِمِينَ وَبَنِي ضَمْرَةَ أَمْنٌ وَسِلْمٌ. وَأَنْ لَا يُنَاصِرُوا أَعْدَاءَ النَّبِيِّ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ . وَإِذَا احْتَاجَ النَّبِيُّ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ إِلَى نُصْرَتِهِمْ، فَإِنَّهُمْ يَنْصُرُونَهُ. وَكَانَ لِوَاءُ الغَزْوَةِ أَبْيَضَ، وَقَدْ حَمَلَهُ حَمْزَةُ بْنُ عَبْدِ الْمُطَّلِبِ رضي الله عنه. وَدَامَتِ الغَزْوَةُ خَمْسَةَ عَشَرَ يَوْمًا، ثُمَّ رَجَعَ رَسُولُ اللهِ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ وَمَنْ مَعَهُ إِلَى الْمَدِينَة.</t>
   </si>
   <si>
     <t>صلح</t>
@@ -185,7 +185,7 @@
     <t>أبي سفيان بن حرب</t>
   </si>
   <si>
-    <t>خَرَجَ الرَّسُولُ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ بِـِمِئَة وَ خَمْسُونَ أَوْ 200 رَجُلٍ لِلْقَاءِ قَافِلَةِ قُرَيْشٍ التِّجَارِيَّةِ الَّتِي ذَهَبَتْ إِلَى الشَّامِ، وَبَلَغُوا مَنْطِقَةَ "ذِي الْعُشَيْرَةِ"، لَكِنَّ الْقَافِلَةَ كَانَتْ قَدْ سَبَقَتْهُمْ بِأَيَّامٍ، فَرَجَعُوا بِدُونِ حَرْبٍ. هَذِهِ الْقَافِلَةُ نَفْسُهَا كَانَتْ سَبَبًا لِخُرُوجِ الْمُسْلِمِينَ فِي غَزْوَةِ بَدْرٍ الْكُبْرَى لَاحِقًا.</t>
+    <t>خَرَجَ الرَّسُولُ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ بِـِمِئَة وَ خَمْسُينَ أَو مئَتَين رَجُلٍ لِلْقَاءِ قَافِلَةِ قُرَيْشٍ التِّجَارِيَّةِ الَّتِي ذَهَبَتْ إِلَى الشَّامِ، وَبَلَغُوا مَنْطِقَةَ "ذِي الْعُشَيْرَةِ"، لَكِنَّ الْقَافِلَةَ كَانَتْ قَدْ سَبَقَتْهُمْ بِأَيَّامٍ، فَرَجَعُوا بِدُونِ حَرْبٍ. هَذِهِ الْقَافِلَةُ نَفْسُهَا كَانَتْ سَبَبًا لِخُرُوجِ الْمُسْلِمِينَ فِي غَزْوَةِ بَدْرٍ الْكُبْرَى لَاحِقًا.</t>
   </si>
   <si>
     <t>اعتراض قافلة قريش التجارية الذاهبة إلى الشام</t>
@@ -575,7 +575,8 @@
     <t>مرحب اليهودي</t>
   </si>
   <si>
-    <t>بَعْدَ عامٍ مِنْ صُلْحِ الحُدَيْبِيَةِ، وتَحْدِيدًا في مُحَرَّمٍ مِنَ السَّنَةِ السَّابِعَةِ لِلهِجْرَةِ، خَرَجَ رَسُولُ اللهِ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ مِنَ المَدِينَةِ فِي نَحْوِ أَلْفٍ وَأَرْبَعِ مِئَةٍ مِنَ الصَّحَابَةِ مُتَوَجِّهِينَ إِلَى واحَةِ خَيْبَرَ شِمالِيَّ الحِجَازِ؛ إِذْ أَصْبَحَتْ حُصُونُ اليَهُودِ هُناكَ مَرْكَزًا لِتَحْرِيضِ القَبَائِلِ ضِدَّ الدَّوْلَةِ الإِسْلَامِيَّةِ وَتَمْوِيلِ الأَعْدَاءِ. وَصَلَ الجَيْشُ لَيْلًا فَأَغْلَقَ أَهْلُ خَيْبَرَ أَبْوَابَهُمْ، فَنَادَى النَّبِيُّ: «اللهُ أَكْبَرُ، خَرِبَتْ خَيْبَرُ!». كانَتِ الواحَةُ سِلْسِلَةَ حُصُونٍ مَوْصُولَةٍ، فَحَاصَرَ المُسْلِمُونَ أَوَّلًا مِنْطَقَةَ «النَّطاةِ» وَفَتَحُوا حِصْنَ «نَعْمٍ» ثُمَّ «الصَّعْبِ بْنِ مُعاذٍ» بَعْدَ قِتالٍ عَنِيفٍ، لِتَنْهَارَ مَعَها مَعْنَوِيَّاتُ المُدافِعِينَ. اِنْتَقَلُوا بَعْدَها إِلَى مِنْطَقَةِ «الشِّقِّ» فَاسْتَسْلَمَ حِصْنُ «الزٌّبَيْرِ»، ثُمَّ تَقَدَّمُوا إِلَى أَقْوَى حُصُونِ خَيْبَرَ وَهُوَ «القَمُوصُ». وفِي صَباحٍ بارِدٍ قالَ رَسُولُ اللهِ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ: «لَأُعْطِيَنَّ الرَّايَةَ غَدًا رَجُلًا يُحِبُّ اللهَ وَرَسُولَهُ وَيُحِبُّهُ اللهُ وَرَسُولُهُ»، فَدَعا عَلِيَّ بْنَ أَبِي طالِبٍ وَهُوَ أَرْمَدُ، فَتَفَلَ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ فِي عَيْنَيْهِ فَبَرِئَ، وَحَمَلَ الرَّايَةَ، وَدَعا اليَهُودَ إِلَى الإِسْلَامِ، فَلَمَّا أَبَوْا بارَزَهُمْ فَقَتَلَ مَرْحَبًا سَيِّدَهُمْ الشَّهِيرَ: «أنا الَّذِي سَمَّتْنِي أُمِّي مَرْحَبُ…»، وَسَقَطَ الحِصْنُ بَعْدَ مُقاوَمَةٍ شَرِسَةٍ. تَوالى سُقُوطُ الحُصُونِ حَتَّى اضْطُرَّ اليَهُودُ لِطَلَبِ الصُّلْحِ، فَوافَقَهُمُ النَّبِيُّ عَلَى البَقاءِ فِي الأَرْضِ يَعْمَلُونَها بِنِصْفِ الثَّمَرَةِ لِلْمُسْلِمِينَ، وَاشْتَرَطَ أَنْ يُخْرِجَهُمْ مَتَى شَاءَ. فِي الطَّرِيقِ عُرِضَتْ عَلَيْهِ صَفِيَّةُ بِنْتُ حُيَيٍّ، فَاصْطَفاها لِنَفْسِهِ وَتَزَوَّجَها، فَكانَتْ أُمَّ المُؤْمِنِينَ. وَبَعْدَ يَوْمَيْنِ قَدَّمَتِ امْرَأَةٌ يَهُودِيَّةٌ شاةً مَسْمُومَةً لِلنَّبِيِّ فَأَكَلَ مِنْها لُقْمَةً وَتَقَيَّأَها، وَماتَ بَعْضُ الصَّحَابَةِ بِالسُّمِّ، فَعَفَا عَنْها ثُمَّ قُتِلَتْ قِصاصًا لاحِقًا. رَجَعَ الجَيْشُ إِلَى المَدِينَةِ مُثْقَلًا بِالغَنائِمِ؛ فَقَسَّمَ رَسُولُ اللهِ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ أَرْبَعَةَ أَخْماسِها عَلَى المُقاتِلِينَ، وَحَبَسَ الخُمُسَ لِمَصارِفِهِ الشَّرْعِيَّةِ، وَأَعْطى مَنْ تَخَلَّفَ مِنْ أَهْلِ الحُدَيْبِيَةِ سِهامًا مِنَ الغَنيمَةِ مَكافَأَةً عَلَى نِيَّتِهِمُ الصَّادِقَةِ. أَسْفَرَتْ خَيْبَرُ عَنْ تَأْمِينِ الجَبْهَةِ الشَّمالِيَّةِ، وَرَفْعِ القُوَّةِ الاقْتِصادِيَّةِ لِلدَّوْلَةِ بِنِصْفِ إِنْتاجِ الواحَةِ، وَتَثْبِيتِ أَمْنِ طَرِيقِ الشَّامِ، كَما فَتَحَتِ البابَ أَمامَ وُفُودِ القَبائِلِ الَّتِي جاءَتْ تُعْلِنُ إِسْلامَها بَعْدَ أَنْ رَأَتْ تَفَوُّقَ المُسْلِمِينَ؛ فَكانَتْ خَيْبَرُ خُطْوَةً حاسِمَةً سَبَقَتْ فَتْحَ مَكَّةَ بِعامٍ واحِدٍ وَرَسَّخَتْ مَكانَةَ الدَّوْلَةِ النُّبُوِيَّةِ فِي الجَزيرَةِ العَرَبِيَّةِ</t>
+    <t>فِي مُحَرَّمٍ مِنَ السَّنَةِ السَّابِعَةِ لِلهِجْرَة، خَرَجَ النَّبِيُّ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ بِأَلْفٍ وَأَرْبَعِ مِئَةٍ إِلَى خَيْبَرَ، حَيْثُ كَانَتْ حُصُونُ الْيَهُودِ مَرْكَزًا لِلتَّحْرِيضِ وَتَمْوِيلِ الأَعْدَاءِ. بَدَأَ الْمُسْلِمُونَ بِحِصَارِ حُصُونِ النَّطَاةِ فَسَقَطَتْ، ثُمَّ تَقَدَّمُوا إِلَى الْقَمُوصِ أَقْوَى الحُصُونِ، فَدَفَعَ النَّبِيُّ الرَّايَةَ لِعَلِيٍّ بْنِ أَبِي طَالِب، فَقَتَلَ مَرْحَبُ وَفُتِحَ الحِصْنُ.
+طَلَبَ الْيَهُودُ الصُّلْحَ، فَوَافَقَ النَّبِيُّ عَلَى أَنْ يَبْقَوْا فِي الأَرْضِ بِنِصْفِ الثَّمَرَةِ. وَفِي الطَّرِيقِ، تَزَوَّجَ صَفِيَّةَ بِنْتَ حُيَيٍّ. ثُمَّ رَجَعَ الجَيْشُ بِغَنَائِمَ كَثِيرَةٍ، وَأَمَّنَتْ خَيْبَرُ الْجَبْهَةَ الشِّمَالِيَّة، وَزَادَتْ قُوَّةَ الدَّوْلَةِ، وَمَهَّدَتْ لِفَتْحِ مَكَّة.</t>
   </si>
   <si>
     <t>تحريض يهود خيبر للقبائل ضد المدينة, كون خيبر مركز تمويل لحلفاء مكة</t>
@@ -605,7 +606,8 @@
     <t>مالك بن رافع الغساني</t>
   </si>
   <si>
-    <t>لَمَّا قُتِلَ الحارِثُ بن عمير الأزْديُّ الذي أرسَلَهُ النّبي صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ بِرِسالةٍ إلى الروم، أجابَ النبيّ بقواتٍ عدَّها نحو ثلاثة آلاف يُمَهِّدُ بها لمعركةٍ كبرى، فأمر زيداً، فإنْ قُتِلَ فجعفراً، فإنْ قُتلَ فعبد الله بن رواحة يحملُ الرّاية. وصَلَ المسلمون إلى مؤتة، فتصدَّر زيدٌ القتالَ فاستشهدَ، ثم جعفرٌ، فابنُ رواحة فَاستُشهد. وعند عودة الجيش، وصف النبيّ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ ذلك نصرًا معنويًا قائلاً: «بل هم الكرّار»، و«حُمِيَ الوَطيسُ» بمعنى اشتدَّ القتالُ، وأقرّ بأنّ المسلمين قد واجَهوا أعداءً كثيرين، وكانَت هذه المعركةُ نقطةَ انطلاقٍ لفَتحِ الشامِ لاحقاً .</t>
+    <t>لَمَّا قُتِلَ الحارِثُ بنُ عُمَيْرٍ الأَزْدِيُّ الَّذِي أَرْسَلَهُ النَّبِيُّ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ بِرِسَالَةٍ إِلَى الرُّومِ، أَجَابَ النَّبِيُّ بِقُوَّاتٍ عَدَّهَا نَحْوَ ثَلَاثَةِ آلَافٍ يُمَهِّدُ بِهَا لِمَعْرَكَةٍ كُبْرَى، فَأَمَرَ زَيْدًا، فَإِنْ قُتِلَ فَجَعْفَرًا، فَإِنْ قُتِلَ فَعَبْدَ اللَّهِ بْنُ رَوَاحَةَ يَحْمِلُ الرَّايَةَ.
+وَصَلَ المُسْلِمُونَ إِلَى مُؤْتَةَ، فَتَصَدَّرَ زَيْدٌ القِتَالَ فَاسْتُشْهِدَ، ثُمَّ جَعْفَرٌ، فَابْنُ رَوَاحَةَ فَاسْتُشْهِدَ. وَعِنْدَ عَوْدَةِ الجَيْشِ، وَصَفَ النَّبِيُّ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ ذَلِكَ نَصْرًا مَعْنَوِيًّا قَائِلًا: بَلْ هُمُ الكَرَّارُ، وَقَالَ: حُمِيَ الوَطِيسُ؛ أَيْ اشْتَدَّ القِتَالُ. وَأَقَرَّ بِأَنَّ المُسْلِمِينَ قَدْ وَاجَهُوا أَعْدَاءً كَثِيرِينَ، وَكَانَتْ هَذِهِ المَعْرَكَةُ نُقْطَةَ انْطِلَاقٍ لِفَتْحِ الشَّامِ لَاحِقًا.</t>
   </si>
   <si>
     <t>قتل شرحبيل ابن عمرو الغساني الحارث بن عمير الأزدي المرسل من النبي، وكسر لحرمة الرسل</t>
@@ -671,7 +673,7 @@
     <t>عبد ياليل بن عمرو الثقفي</t>
   </si>
   <si>
-    <t>بعدَ غزوةِ حُنَيْنٍ، قرّرَ النبيُّ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ أنْ يتّجهَ إلى الطّائفِ، وهي من المناطقِ المُهمّةِ في جنوبِ الجزيرةِ العربيّةِ، وذلكَ لمحاولةِ نشرِ الإسلامِ هناكَ، وإقناعِ أهلِها بالانضمامِ إلى المسلمينَ. خرجَ مع أصحابِهِ في رحلةٍ طويلةٍ، ولكنّ أهلَ الطّائفِ قاوموا مقاومةً عنيفةً، خاصّةً قبيلةُ هَوازِن، التي كانتْ من أكبرِ قبائلِ المنطقةِ. واجهَ النبيُّ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ مقاومةً شرسةً، ووقعتْ بعضُ المعاركِ الصغيرةِ، وأُصيبَ بجراحٍ بالغةٍ، كما أُصيبَ بعضُ أصحابِهِ كذلكَ.حاولَ النبيُّ أنْ يُهدّئَ من مقاومةِ أهلِ الطّائفِ، لكنّه لم ينجحْ في فَرضِ السّيطرةِ الكاملةِ. هذه الغزوةُ لم تكنْ حاسمةً، لكنها كانتْ محاوَلةً مُهِمّةً لنشرِ الإسلامِ في جنوبِ الجزيرةِ، وأظهرتْ أنّ الدّعوةَ تُواجهُ تحدّياتٍ كبيرةً، وأنّ المقاومةَ كانتْ عنيفةً.</t>
+    <t>بعدَ غزوةِ حُنَيْنٍ، قرّرَ النبيُّ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ أنْ يتّجهَ إلى الطّائفِ، وهي من المناطقِ المُهمّةِ في جنوبِ الجزيرةِ العربيّةِ، وذلكَ لمحاولةِ نشرِ الإسلامِ، وإقناعِ أهلِها بالانضمامِ إلى المسلمينَ. خرجَ مع أصحابِهِ في رحلةٍ طويلةٍ، ولكنّ أهلَ الطّائفِ قاوموا مقاومةً عنيفةً، خاصّةً قبيلةُ هَوازِن، التي كانتْ من أكبرِ قبائلِ المنطقةِ. واجهَ النبيُّ صَلَّى اللَّهُ عَلَيْهِ وَسَلَّمَ مقاومةً شرسة، ووقعتْ بعضُ المعاركِ الصغيرةِ، وأُصيبَ بجراحٍ بالغةٍ، كما أُصيبَ بعضُ أصحابِهِ كذلكَ.حاولَ النبيُّ أنْ يُهدّئَ من مقاومةِ أهلِ الطّائفِ، لكنّه لم ينجحْ في فَرضِ السّيطرةِ الكاملةِ. هذه الغزوةُ لم تكنْ حاسمةً، لكنها كانتْ محاوَلةً مُهِمّةً لنشرِ الإسلامِ في جنوبِ الجزيرةِ، وأظهرتْ أنّ الدّعوةَ تُواجهُ تحدّياتٍ كبيرةً، وأنّ المقاومةَ كانتْ عنيفةً.</t>
   </si>
   <si>
     <t>تحصن فلول الكفار من غزوة حنين داخل الطائف</t>
@@ -770,7 +772,7 @@
     <t>قافلة لقريش متجهة إلى الشام</t>
   </si>
   <si>
-    <t>هِيَ مَعْرَكَةٌ وَقَعَت بَيْنَ خَالِدِ بْنِ الوَلِيدِ وَجَيْشِ الزَّرَاحَةِ الَّذِينَ نَجَوْا مِنْ مَعْرَكَةِ بُزَاخَةَ. وَقَدْ جَرَتْ فِي مَوْقِعٍ يُسَمَّى غَمْرَةَ، يَبْعُدُ نَحْوَ 20 مِيلًا عَنْ بُزَاخَةَ (فِي السُّعُودِيَّةِ حَالِيًّا). انْتَهَتِ المَعْرَكَةُ بِانْتِصَارِ جَيْشِ الخِلَافَةِ الرَّاشِدَةِ، وَكَانَ ذَلِكَ نَصْرًا حَاسِمًا لِلْمُسْلِمِينَ.</t>
+    <t>هِيَ مَعْرَكَةٌ وَقَعَت بَيْنَ خَالِدِ بْنِ الوَلِيدِ وَجَيْشِ الزَّرَاحَةِ الَّذِينَ نَجَوْا مِنْ مَعْرَكَةِ بُزَاخَة. وَقَدْ جَرَتْ فِي مَوْقِعٍ يُسَمَّى غَمْرَةَ، يَبْعُدُ نَحْوَ عشرون مِيلًا عَنْ بُزَاخَة (فِي السُّعُودِيَّةِ حَالِيًّا). انْتَهَتِ المَعْرَكَةُ بِانْتِصَارِ جَيْشِ الخِلَافَةِ الرَّاشِدَةِ، وَكَانَ ذَلِكَ نَصْرًا حَاسِمًا لِلْمُسْلِمِينَ.</t>
   </si>
   <si>
     <t>ردع المرتدين في الجيش المتبغي من معركة بزاخة</t>
@@ -851,7 +853,7 @@
     <t>مبهوذان</t>
   </si>
   <si>
-    <t>لَمَّا انْتَهَتْ مَعْرَكَةُ الحُصَيْدِ بِنَصْرٍ لِلْمُسْلِمِينَ، هَرَبَتْ فُلُولُ الفُرْسِ وَمَنْ تَحَالَفَ مَعَهُمْ مِنَ العَرَبِ النَّصَارَى نَحْوَ مَكَانٍ يُسَمَّى الخَنَافِس، وَهُوَ سُوقٌ عَرِيقٌ كَانَ يَقَعُ قُرْبَ الفُرَاتِ فِي أَرْضِ العِرَاقِ. كَانَ الْهَارِبُونَ يَرْجُونَ أَنْ يُعِيدُوا تَجْمِيعَ صُفُوفِهِمْ، وَيَحْصُلُوا عَلَى مَدَدٍ يُعِيدُ لَهُمْ رُوحَ القِتَالِ، وَيُمَكِّنُهُمْ مِنَ التَّصَدِّي لِجُيُوشِ الإِسْلَامِ.وَكَانَ عَلَى رَأْسِ الْمُسْلِمِينَ فِي تِلْكَ الْجِهَةِ القَائِدُ الْمِقْدَامُ عُرْوَةُ بْنُ الجَعْدِ البَارِقِيُّ، وَهُوَ صَحَابِيٌّ شُجَاعٌ، تَلَقَّى أَمْرَهُ مِنَ القَائِدِ الأَعْلَى خَالِدِ بْنِ الوَلِيدِ، بِأَنْ يُلاحِقَ الْهَارِبِينَ، وَيَضْرِبَ عَلَيْهِمْ طَوْقًا، حَتَّى لا يُفْلِتُوا وَلَا يَجْمَعُوا جَيْشًا جَدِيدًا.فِي لَيْلَةٍ سَاكِنَةٍ، وَبَعْدَ سُرْعَةِ مَسِيرٍ عَجُولٍ، وَصَلَ عُرْوَةُ بْنُ الجَعْدِ بِفِرْقَتِهِ إِلَى أَطْرَافِ سُوقِ الخَنَافِسِ. كَانَتِ الرِّيحُ تَهُبُّ عَلَى رِكَامِ التِّجَارَةِ، وَلَا أَثَرَ لِجُنْدٍ وَلَا قِتَالٍ. تَرَيَّثَ الْجَيْشُ قَلِيلًا، حَذَرًا مِنْ كَمِينٍ، ثُمَّ تَقَدَّمُوا بِحَذَرٍ، لِيَجِدُوا السُّوقَ خَالِيًا إِلَّا مِنْ آثَارِ هُرُوبٍ وَفَرَارٍ.اتَّضَحَ لَهُمْ أَنَّ الفُرْسَ وَحُلَفَاءَهُمْ قَدْ فَرُّوا دُونَ قِتَالٍ، تَارِكِينَ المَكَانَ فَارِغًا، تَخْنُقُهُ رَوَائِحُ التُّرَابِ وَالأَمْوَالِ الْمُهْمَلَةِ. دَخَلَ المُسْلِمُونَ السُّوقَ، وَأَقَامُوا فِيهِ، وَجَمَعُوا مَا خَلَّفَهُ العَدُوُّ، وَكَانَ فَتْحًا بِلَا سَيْفٍ وَلَا دِمَاء، لَكِنَّهُ كَانَ ضَرْبَةً نَفْسِيَّةً قَاصِمَةً لِلْفُرْسِ، وَانْتِصَارًا مَعْنَوِيًّا كَبِيرًا لِلْمُسْلِمِينَ.وَبِذَلِكَ كَانَ فَتْحُ الخَنَافِسِ مِنَ الفُتُوحِ الَّتِي لَمْ يُرْفَعْ فِيهَا سَيْفٌ، وَلَكِنْ أَرْعَبَتِ الأَعْدَاءَ، وَثَبَّتَتْ أَقْدَامَ الإِسْلَامِ فِي مَجَالٍ جَدِيدٍ، وَفَتَحَتِ الطَّرِيقَ لِمَعَارِكِ أُخْرَى أَشَدَّ وَأَعْنَفَ فِي طَرِيقِ فَتْحِ العِرَاقِ وَفَارِس.</t>
+    <t>لَمَّا انْتَهَتْ مَعْرَكَةُ الحُصَيْدِ بِنَصْرٍ لِلْمُسْلِمِينَ، فَرَّتْ فُلُولُ الفُرْسِ وَحُلَفَاؤُهُمْ نَحْوَ سُوقِ الخَنَافِسِ قُرْبَ الفُرَاتِ، أَمَلًا فِي إِعَادَةِ التَّجْمِيعِ. أَمَرَ خَالِدُ بْنُ الوَلِيدِ القَائِدَ عُرْوَةَ بْنَ الجَعْدِ بِمُطَارَدَتِهِمْ، فَانْطَلَقَ لَيْلًا حَتَّى بَلَغَ السُّوقَ، فَوَجَدَهُ خَالِيًا إِلَّا مِنْ آثَارِ الفِرَارِ. لَمْ يَجْرِ قِتَالٌ، وَدَخَلَ المُسْلِمُونَ السُّوقَ وَجَمَعُوا مَا خَلَّفَهُ العَدُوُّ. فَكَانَ فَتْحُ الخَنَافِسِ نَصْرًا نَفْسِيًّا بِلَا دِمَاء، أَرْعَبَ الفُرْسَ وَمَهَّدَ الطَّرِيقَ لِفُتُوحِ العِرَاقِ.</t>
   </si>
   <si>
     <t>فلول الجيش الفارسي المنهزم في معركة حصيد تفر إلى الخنافس</t>
@@ -2087,7 +2089,7 @@
     <t>شهربراز جاذویه</t>
   </si>
   <si>
-    <t>في سَنةِ واحد وعشرون للهجرة، ضِمنَ سِلسِلةِ الفُتوحِ بعدَ مَعركةِ نَهاوَند، مَرَّرَ الخليفةُ عُمرُ بنُ الخَطّابِ بمرحلةٍ مُهِمّةٍ لِتنظيمِ السَّيطرةِ الإسلاميّةِ على وَسَطِ فَارِس. فأَمَرَ بإرسالِ عَبدِ اللهِ بنِ عَبدِ اللهِ بنِ عُتبان – مَدعومًا بأبي مُوسى الأَشعَري – إلى أصفَهان، التي لم تُخضَع بَعدُ رغمَ سُقوطِ المُدنِ المُجاوِرة, واجَهَ الجَيشُ الإسلاميُّ القُوّاتِ الفارسيّةَ في خَراجِ المدينةِ وما حَولَها، وتمكَّنَ عبدُ اللهِ بنُ عُتبانَ من قَتلِ قائدِ الفُرسِ في المُبارَزة. ثم بَدأَ حِصارًا استمرَّ عِدّةَ أَشهُر، حتّى رَضَخَ أهلُ أصفَهانَ ووقَّعوا الصُّلحَ على الجِزيَةِ وحُكمِ الدَّولةِ الإسلاميّة.</t>
+    <t>في سَنةِ واحد وعشرون للهجرة، ضِمنَ سِلسِلةِ الفُتوحِ بعدَ مَعركةِ نَهاوَند، مَرَّ الخليفةُ عُمرُ بنُ الخَطّابِ بمرحلةٍ مُهِمّةٍ لِتنظيمِ السَّيطرةِ الإسلاميّةِ على وَسَطِ فَارِس. فأَمَرَ بإرسالِ عَبدِ اللهِ بنِ عَبدِ اللهِ بنِ عُتبان – مَدعومًا بأبي مُوسى الأَشعَري – إلى أصفَهان، التي لم تُخضَع بَعدُ رغمَ سُقوطِ المُدنِ المُجاوِرة, واجَهَ الجَيشُ الإسلاميُّ القُوّاتِ الفارسيّةَ في خَراجِ المدينةِ وما حَولَها، وتمكَّنَ عبدُ اللهِ بنُ عُتبانَ من قَتلِ قائدِ الفُرسِ في المُبارَزة. ثم بَدأَ حِصارًا استمرَّ عِدّةَ أَشهُر، حتّى رَضَخَ أهلُ أصفَهانَ ووقَّعوا الصُّلحَ على الجِزيَةِ وحُكمِ الدَّولةِ الإسلاميّة.</t>
   </si>
   <si>
     <t>القضاء النهائي على النفوذ الفارسي في مناطق وسط إيران، وحماية المناطق المحررة من أي انكفاء أو تمرد, أمر الخليفة عمر بن الخطاب بإرسال جيش بقيادة عبد الله بن عبد الله بن عتبان لتعزيز الفتح، وتحصين السيطرة بنيّة تحويل هذه المدن إلى مراكز إسلامية مستقرة</t>
@@ -2877,7 +2879,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2932,7 +2934,6 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3160,8 +3161,8 @@
   </sheetPr>
   <dimension ref="A1:AD1033"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4350,7 +4351,7 @@
       <c r="K24" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="L24" s="30" t="s">
+      <c r="L24" s="29" t="s">
         <v>178</v>
       </c>
       <c r="M24" s="3" t="s">
@@ -4399,7 +4400,7 @@
       <c r="K25" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="L25" s="30" t="s">
+      <c r="L25" s="29" t="s">
         <v>188</v>
       </c>
       <c r="M25" s="9" t="s">
@@ -4520,7 +4521,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:30" ht="150.75">
+    <row r="28" spans="1:30" ht="138.75">
       <c r="A28" s="16" t="s">
         <v>206</v>
       </c>
@@ -4791,7 +4792,7 @@
       <c r="AC32" s="6"/>
       <c r="AD32" s="6"/>
     </row>
-    <row r="33" spans="1:30" ht="12.6">
+    <row r="33" spans="1:30" ht="58.5">
       <c r="A33" s="15" t="s">
         <v>246</v>
       </c>
@@ -4819,7 +4820,7 @@
       <c r="K33" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="L33" s="30" t="s">
+      <c r="L33" s="29" t="s">
         <v>250</v>
       </c>
       <c r="M33" s="3" t="s">
@@ -4838,7 +4839,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="34" spans="1:30" ht="12.6">
+    <row r="34" spans="1:30" ht="69">
       <c r="A34" s="15" t="s">
         <v>254</v>
       </c>
@@ -4866,7 +4867,7 @@
       <c r="K34" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="L34" s="30" t="s">
+      <c r="L34" s="29" t="s">
         <v>259</v>
       </c>
       <c r="M34" s="3" t="s">
@@ -4885,7 +4886,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="35" spans="1:30" ht="12.6">
+    <row r="35" spans="1:30" ht="81">
       <c r="A35" s="15" t="s">
         <v>263</v>
       </c>
@@ -4915,7 +4916,7 @@
       <c r="K35" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="L35" s="30" t="s">
+      <c r="L35" s="29" t="s">
         <v>270</v>
       </c>
       <c r="M35" s="3" t="s">
@@ -4983,7 +4984,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="37" spans="1:30" ht="12.6">
+    <row r="37" spans="1:30" ht="219.75">
       <c r="A37" s="15" t="s">
         <v>281</v>
       </c>
@@ -5013,7 +5014,7 @@
       <c r="K37" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L37" s="30" t="s">
+      <c r="L37" s="29" t="s">
         <v>284</v>
       </c>
       <c r="M37" s="3" t="s">
@@ -5032,7 +5033,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="38" spans="1:30" ht="12.6">
+    <row r="38" spans="1:30" ht="150.75">
       <c r="A38" s="15" t="s">
         <v>287</v>
       </c>
@@ -5062,7 +5063,7 @@
       <c r="K38" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="L38" s="30" t="s">
+      <c r="L38" s="29" t="s">
         <v>291</v>
       </c>
       <c r="M38" s="3" t="s">
@@ -5143,7 +5144,7 @@
       <c r="AC39" s="6"/>
       <c r="AD39" s="6"/>
     </row>
-    <row r="40" spans="1:30" ht="12.6">
+    <row r="40" spans="1:30" ht="58.5">
       <c r="A40" s="15" t="s">
         <v>300</v>
       </c>
@@ -5175,7 +5176,7 @@
       <c r="K40" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="L40" s="30" t="s">
+      <c r="L40" s="29" t="s">
         <v>306</v>
       </c>
       <c r="M40" s="3" t="s">
@@ -5593,7 +5594,7 @@
       <c r="K48" s="19" t="s">
         <v>377</v>
       </c>
-      <c r="L48" s="31" t="s">
+      <c r="L48" s="30" t="s">
         <v>378</v>
       </c>
       <c r="M48" s="3" t="s">
@@ -6478,7 +6479,7 @@
       <c r="K65" s="3" t="s">
         <v>503</v>
       </c>
-      <c r="L65" s="32" t="s">
+      <c r="L65" s="31" t="s">
         <v>504</v>
       </c>
       <c r="M65" s="3" t="s">
@@ -7484,7 +7485,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="85" spans="1:17" ht="12.75">
+    <row r="85" spans="1:17" ht="81">
       <c r="A85" s="24" t="s">
         <v>647</v>
       </c>
@@ -7518,7 +7519,7 @@
       <c r="K85" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L85" s="3" t="s">
+      <c r="L85" s="14" t="s">
         <v>652</v>
       </c>
       <c r="M85" s="3" t="s">
@@ -7641,7 +7642,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="88" spans="1:17" ht="12.75">
+    <row r="88" spans="1:17" ht="104.25">
       <c r="A88" s="24" t="s">
         <v>672</v>
       </c>
@@ -7671,7 +7672,7 @@
       <c r="K88" s="3" t="s">
         <v>675</v>
       </c>
-      <c r="L88" s="3" t="s">
+      <c r="L88" s="14" t="s">
         <v>676</v>
       </c>
       <c r="M88" s="3" t="s">
@@ -7743,7 +7744,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="90" spans="1:17" ht="12.75">
+    <row r="90" spans="1:17" ht="69">
       <c r="A90" s="24" t="s">
         <v>688</v>
       </c>
@@ -7773,7 +7774,7 @@
       <c r="K90" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L90" s="3" t="s">
+      <c r="L90" s="14" t="s">
         <v>691</v>
       </c>
       <c r="M90" s="3" t="s">

</xml_diff>